<commit_message>
Further temporary renaming workaround attempts
</commit_message>
<xml_diff>
--- a/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
+++ b/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
@@ -25340,20 +25340,21 @@
     </x:row>
     <x:row r="1421">
       <x:c r="A1421" s="2" t="str">
-        <x:v>MatrixElement</x:v>
+        <x:v>Matri</x:v>
       </x:c>
       <x:c r="B1421" s="2" t="str">
-        <x:v>EXTENSION-MatrixElement</x:v>
+        <x:v>EXTENSION-Matri</x:v>
       </x:c>
       <x:c r="C1421" s="2" t="str">
-        <x:v>EXTENSION-Matrixx</x:v>
+        <x:v>EXTENSION-SurveyQuestion</x:v>
       </x:c>
       <x:c r="D1421" s="2" t="str">
         <x:v>minOccurs: 0
+maxOccurs: unbounded
 </x:v>
       </x:c>
       <x:c r="E1421" s="2" t="str">
-        <x:v>For matrix questions, the text identifying each row of the matrix.</x:v>
+        <x:v>(TPDP Extension) Information about the matrix element in the survey</x:v>
       </x:c>
     </x:row>
     <x:row r="1422">
@@ -25375,21 +25376,20 @@
     </x:row>
     <x:row r="1423">
       <x:c r="A1423" s="2" t="str">
-        <x:v>Matrixx</x:v>
+        <x:v>MatrixElement</x:v>
       </x:c>
       <x:c r="B1423" s="2" t="str">
-        <x:v>EXTENSION-Matrixx</x:v>
+        <x:v>EXTENSION-MatrixElement</x:v>
       </x:c>
       <x:c r="C1423" s="2" t="str">
-        <x:v>EXTENSION-SurveyQuestion</x:v>
+        <x:v>EXTENSION-Matri</x:v>
       </x:c>
       <x:c r="D1423" s="2" t="str">
         <x:v>minOccurs: 0
-maxOccurs: unbounded
 </x:v>
       </x:c>
       <x:c r="E1423" s="2" t="str">
-        <x:v>(TPDP Extension) Information about the matrix element in the survey</x:v>
+        <x:v>For matrix questions, the text identifying each row of the matrix.</x:v>
       </x:c>
     </x:row>
     <x:row r="1424">
@@ -25562,7 +25562,7 @@
         <x:v>xs:int</x:v>
       </x:c>
       <x:c r="C1433" s="2" t="str">
-        <x:v>EXTENSION-Matrixx</x:v>
+        <x:v>EXTENSION-Matri</x:v>
       </x:c>
       <x:c r="D1433" s="2" t="str">
         <x:v>minOccurs: 0
@@ -25915,7 +25915,7 @@
         <x:v>xs:int</x:v>
       </x:c>
       <x:c r="C1452" s="2" t="str">
-        <x:v>EXTENSION-Matrixx</x:v>
+        <x:v>EXTENSION-Matri</x:v>
       </x:c>
       <x:c r="D1452" s="2" t="str">
         <x:v>minOccurs: 0
@@ -47815,7 +47815,7 @@
     </x:row>
     <x:row r="297">
       <x:c r="A297" s="2" t="str">
-        <x:v>EXTENSION-Matrixx</x:v>
+        <x:v>EXTENSION-Matri</x:v>
       </x:c>
       <x:c r="B297" s="2" t="str">
         <x:v>Information about the matrix element in the survey</x:v>

</xml_diff>

<commit_message>
Proof reading changes continued
</commit_message>
<xml_diff>
--- a/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
+++ b/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
@@ -2895,7 +2895,7 @@
         <x:v/>
       </x:c>
       <x:c r="E157" s="2" t="str">
-        <x:v>The average of the numeric responses to survey sections collected at the aggregate level.</x:v>
+        <x:v>The information about the numeric response for an aggregated survey.</x:v>
       </x:c>
     </x:row>
     <x:row r="158">
@@ -4287,7 +4287,7 @@
         <x:v/>
       </x:c>
       <x:c r="E235" s="2" t="str">
-        <x:v>The Anonymized Student reference for the association</x:v>
+        <x:v>The Anonymized Student reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="236">
@@ -4321,7 +4321,7 @@
         <x:v/>
       </x:c>
       <x:c r="E237" s="2" t="str">
-        <x:v>The Anonymozed Student reference for the association</x:v>
+        <x:v>The Anonymized Student reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="238">
@@ -4338,7 +4338,7 @@
         <x:v/>
       </x:c>
       <x:c r="E238" s="2" t="str">
-        <x:v>The Anonymized Student reference for the association</x:v>
+        <x:v>The Anonymized Student reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="239">
@@ -4406,7 +4406,7 @@
         <x:v/>
       </x:c>
       <x:c r="E242" s="2" t="str">
-        <x:v>The Anonymozed Student reference for the association</x:v>
+        <x:v>The Anonymized Student reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="243">
@@ -4423,7 +4423,7 @@
         <x:v/>
       </x:c>
       <x:c r="E243" s="2" t="str">
-        <x:v>The Anonymized Student reference for the association</x:v>
+        <x:v>The Anonymized Student reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="244">
@@ -4440,7 +4440,7 @@
         <x:v/>
       </x:c>
       <x:c r="E244" s="2" t="str">
-        <x:v>The Anonymized Student reference for the association</x:v>
+        <x:v>The Anonymized Student reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="245">
@@ -5009,7 +5009,7 @@
 </x:v>
       </x:c>
       <x:c r="E275" s="2" t="str">
-        <x:v>The category of an assessment based on format and content. For example: Achievement test Advanced placement test Alternate assessment/grade-level standards Attitudinal test Cognitive and perceptual skills test ...</x:v>
+        <x:v>The category of an assessment based on format and content. For example: Achievement test, Advanced placement, Alternate assessment/grade-level standards, Attitudinal test, Cognitive and perceptual skills test.</x:v>
       </x:c>
     </x:row>
     <x:row r="276">
@@ -5129,7 +5129,7 @@
 </x:v>
       </x:c>
       <x:c r="E281" s="2" t="str">
-        <x:v>The category of an assessment based on format and content. For example: Achievement test Advanced placement test Alternate assessment/grade-level standards Attitudinal test Cognitive and perceptual skills test ...</x:v>
+        <x:v>The category of an assessment based on format and content. For example: Achievement test, Advanced placement, Alternate assessment/grade-level standards, Attitudinal test, Cognitive and perceptual skills test.</x:v>
       </x:c>
     </x:row>
     <x:row r="282">
@@ -5147,7 +5147,7 @@
 </x:v>
       </x:c>
       <x:c r="E282" s="2" t="str">
-        <x:v>The category of an assessment based on format and content. For example: Achievement test Advanced placement test Alternate assessment/grade-level standards Attitudinal test Cognitive and perceptual skills test ...</x:v>
+        <x:v>The category of an assessment based on format and content. For example: Achievement test, Advanced placement, Alternate assessment/grade-level standards, Attitudinal test, Cognitive and perceptual skills test.</x:v>
       </x:c>
     </x:row>
     <x:row r="283">
@@ -5920,7 +5920,7 @@
 </x:v>
       </x:c>
       <x:c r="E325" s="2" t="str">
-        <x:v>The title if any specific assessment given to a group</x:v>
+        <x:v>The title of any specific assessment given to a group.</x:v>
       </x:c>
     </x:row>
     <x:row r="326">
@@ -5938,7 +5938,7 @@
 </x:v>
       </x:c>
       <x:c r="E326" s="2" t="str">
-        <x:v>The title if any specific assessment given to a group</x:v>
+        <x:v>The title of a specific assessment given to a group.</x:v>
       </x:c>
     </x:row>
     <x:row r="327">
@@ -5956,7 +5956,7 @@
 </x:v>
       </x:c>
       <x:c r="E327" s="2" t="str">
-        <x:v>The title if any specific assessment given to a group</x:v>
+        <x:v>The title of a specific assessment given to a group.</x:v>
       </x:c>
     </x:row>
     <x:row r="328">
@@ -8400,7 +8400,7 @@
 </x:v>
       </x:c>
       <x:c r="E465" s="2" t="str">
-        <x:v>Board certification information for a individual.</x:v>
+        <x:v>Board certification information for an individual.</x:v>
       </x:c>
     </x:row>
     <x:row r="466">
@@ -8418,7 +8418,7 @@
 </x:v>
       </x:c>
       <x:c r="E466" s="2" t="str">
-        <x:v>An indication of whether a individual is board certified.</x:v>
+        <x:v>An indication of whether an individual is board certified.</x:v>
       </x:c>
     </x:row>
     <x:row r="467">
@@ -8757,7 +8757,7 @@
 </x:v>
       </x:c>
       <x:c r="E485" s="2" t="str">
-        <x:v>Certification information for a individual.</x:v>
+        <x:v>Certification information for an individual.</x:v>
       </x:c>
     </x:row>
     <x:row r="486">
@@ -8809,7 +8809,7 @@
 </x:v>
       </x:c>
       <x:c r="E488" s="2" t="str">
-        <x:v>The type of certification exam that taken.</x:v>
+        <x:v>The type of certification exam that was taken.</x:v>
       </x:c>
     </x:row>
     <x:row r="489">
@@ -11047,7 +11047,7 @@
         <x:v/>
       </x:c>
       <x:c r="E614" s="2" t="str">
-        <x:v>The Course reference for the assocation</x:v>
+        <x:v>The Course reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="615">
@@ -11098,7 +11098,7 @@
         <x:v/>
       </x:c>
       <x:c r="E617" s="2" t="str">
-        <x:v>The Course reference for the assocation</x:v>
+        <x:v>The Course reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="618">
@@ -11626,7 +11626,7 @@
         <x:v/>
       </x:c>
       <x:c r="E647" s="2" t="str">
-        <x:v>The official Course Title with which this student acaemic is associated.</x:v>
+        <x:v>The descriptive name given to a course of study offered in a school or other institution or organization.</x:v>
       </x:c>
     </x:row>
     <x:row r="648">
@@ -13387,7 +13387,7 @@
         <x:v/>
       </x:c>
       <x:c r="E745" s="2" t="str">
-        <x:v>Data about the disability of a group</x:v>
+        <x:v>Data about the disability of a group.</x:v>
       </x:c>
     </x:row>
     <x:row r="746">
@@ -15689,7 +15689,7 @@
         <x:v/>
       </x:c>
       <x:c r="E876" s="2" t="str">
-        <x:v>The Education Organization reference for the assocation</x:v>
+        <x:v>The Education Organization reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="877">
@@ -15894,7 +15894,7 @@
         <x:v/>
       </x:c>
       <x:c r="E888" s="2" t="str">
-        <x:v>The Education Organization reference for the assocation</x:v>
+        <x:v>The Education Organization reference for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="889">
@@ -16082,7 +16082,7 @@
         <x:v/>
       </x:c>
       <x:c r="E899" s="2" t="str">
-        <x:v>The Education Organization Student Academic Record Fact the data is associated with</x:v>
+        <x:v>The Education Organization the course transcript data is associated with.</x:v>
       </x:c>
     </x:row>
     <x:row r="900">
@@ -16099,7 +16099,7 @@
         <x:v/>
       </x:c>
       <x:c r="E900" s="2" t="str">
-        <x:v>The Education Organization Student Academic Record Fact the data is associated with</x:v>
+        <x:v>The Education Organization the course transcript data is associated with.</x:v>
       </x:c>
     </x:row>
     <x:row r="901">
@@ -16674,7 +16674,7 @@
 </x:v>
       </x:c>
       <x:c r="E932" s="2" t="str">
-        <x:v>The number of student who are ELL</x:v>
+        <x:v>The number of students who are ELL.</x:v>
       </x:c>
     </x:row>
     <x:row r="933">
@@ -17124,7 +17124,7 @@
 </x:v>
       </x:c>
       <x:c r="E956" s="2" t="str">
-        <x:v>The end date for the assocation</x:v>
+        <x:v>The end date for the association.</x:v>
       </x:c>
     </x:row>
     <x:row r="957">
@@ -17852,7 +17852,7 @@
 </x:v>
       </x:c>
       <x:c r="E997" s="2" t="str">
-        <x:v>The number of student who are ESL</x:v>
+        <x:v>The number of students who are ESL.</x:v>
       </x:c>
     </x:row>
     <x:row r="998">
@@ -20296,7 +20296,7 @@
 </x:v>
       </x:c>
       <x:c r="E1138" s="2" t="str">
-        <x:v>The final GPA for the teacher achieved in the program.</x:v>
+        <x:v>The final GPA the teacher achieved in the program.</x:v>
       </x:c>
     </x:row>
     <x:row r="1139">
@@ -21873,7 +21873,7 @@
 </x:v>
       </x:c>
       <x:c r="E1227" s="2" t="str">
-        <x:v>The percentage of student who are identified as hispanic/latino</x:v>
+        <x:v>The percentage of students who are identified as hispanic/latino.</x:v>
       </x:c>
     </x:row>
     <x:row r="1228">
@@ -21981,7 +21981,7 @@
 </x:v>
       </x:c>
       <x:c r="E1233" s="2" t="str">
-        <x:v>he hours the staff was absence if not the entire working day</x:v>
+        <x:v>The hours the staff was absent if not the entire working day.</x:v>
       </x:c>
     </x:row>
     <x:row r="1234">
@@ -23802,7 +23802,7 @@
 </x:v>
       </x:c>
       <x:c r="E1335" s="2" t="str">
-        <x:v>The number of student by each lanugage type</x:v>
+        <x:v>The number of students by each language type.</x:v>
       </x:c>
     </x:row>
     <x:row r="1336">
@@ -23820,7 +23820,7 @@
 </x:v>
       </x:c>
       <x:c r="E1336" s="2" t="str">
-        <x:v>The percentage of student by language type</x:v>
+        <x:v>The percentage of students by language type.</x:v>
       </x:c>
     </x:row>
     <x:row r="1337">
@@ -24619,7 +24619,7 @@
 </x:v>
       </x:c>
       <x:c r="E1380" s="2" t="str">
-        <x:v>The percentage of student receiving a letter grade by type</x:v>
+        <x:v>The percentage of students receiving a letter grade by type.</x:v>
       </x:c>
     </x:row>
     <x:row r="1381">
@@ -26924,7 +26924,7 @@
 </x:v>
       </x:c>
       <x:c r="E1509" s="2" t="str">
-        <x:v>The total number of student enrolled in the respective Section</x:v>
+        <x:v>The total number of students enrolled in the respective Section.</x:v>
       </x:c>
     </x:row>
     <x:row r="1510">
@@ -28472,7 +28472,7 @@
 </x:v>
       </x:c>
       <x:c r="E1595" s="2" t="str">
-        <x:v>The percentage of student who met the performance level</x:v>
+        <x:v>The percentage of students who met the performance level.</x:v>
       </x:c>
     </x:row>
     <x:row r="1596">
@@ -28508,7 +28508,7 @@
 </x:v>
       </x:c>
       <x:c r="E1597" s="2" t="str">
-        <x:v>The percentage of student who achieved perfromance level by each performance level type</x:v>
+        <x:v>The percentage of students who achieved performance level by each performance level type.</x:v>
       </x:c>
     </x:row>
     <x:row r="1598">
@@ -29823,7 +29823,7 @@
 </x:v>
       </x:c>
       <x:c r="E1670" s="2" t="str">
-        <x:v>An indication of whether a teacher candidate has completed the teacher prepartion program.</x:v>
+        <x:v>An indication of whether a teacher candidate has completed the teacher preparation program.</x:v>
       </x:c>
     </x:row>
     <x:row r="1671">
@@ -30964,7 +30964,7 @@
         <x:v/>
       </x:c>
       <x:c r="E1735" s="2" t="str">
-        <x:v>The form of question: 1) Radio box: multiple choice, single selection; 2) Checkbox: Multiple choice, multiple selection; 3) Dropdown: multiple choice, single selection; 4) Matrix, numeric rating scale; 5) Matrix of dropdowns; 6) Ranking; 7) Single textbox; 8) Matrix of text boxes.</x:v>
+        <x:v>The form of question: 1) Radio box: multiple choice, single selection; 2) Checkbox: Multiple choice, multiple selection; 3) Dropdown: multiple choice, single selection; 4) Matrix, numeric rating scale; 5) Matrix of dropdowns; 6) Ranking; 7) Single textbook; 8) Matrix of text boxes</x:v>
       </x:c>
     </x:row>
     <x:row r="1736">
@@ -31591,7 +31591,7 @@
 </x:v>
       </x:c>
       <x:c r="E1769" s="2" t="str">
-        <x:v>The information about the recommenation for the credential.</x:v>
+        <x:v>The information about the recommendation for the credential.</x:v>
       </x:c>
     </x:row>
     <x:row r="1770">
@@ -31981,7 +31981,7 @@
 </x:v>
       </x:c>
       <x:c r="E1790" s="2" t="str">
-        <x:v>An indication of whether a teacher candidate is active in an professional development.</x:v>
+        <x:v>An indication of whether a teacher candidate is active in a professional development.</x:v>
       </x:c>
     </x:row>
     <x:row r="1791">
@@ -33081,7 +33081,7 @@
 </x:v>
       </x:c>
       <x:c r="E1852" s="2" t="str">
-        <x:v>The maximum salary range for a staff.</x:v>
+        <x:v>The maximum value in a salary range for staff.</x:v>
       </x:c>
     </x:row>
     <x:row r="1853">
@@ -33117,7 +33117,7 @@
 </x:v>
       </x:c>
       <x:c r="E1854" s="2" t="str">
-        <x:v>The minimum salary range for a staff.</x:v>
+        <x:v>The minimum value in a salary range for staff.</x:v>
       </x:c>
     </x:row>
     <x:row r="1855">
@@ -36630,7 +36630,7 @@
 </x:v>
       </x:c>
       <x:c r="E2054" s="2" t="str">
-        <x:v>The percentage of student by each sex type</x:v>
+        <x:v>The percentage of students by each sex type.</x:v>
       </x:c>
     </x:row>
     <x:row r="2055">
@@ -36862,7 +36862,7 @@
 </x:v>
       </x:c>
       <x:c r="E2067" s="2" t="str">
-        <x:v>The percentage of student enrolled in a SPED program</x:v>
+        <x:v>The percentage of students enrolled in a SPED program.</x:v>
       </x:c>
     </x:row>
     <x:row r="2068">
@@ -38934,7 +38934,7 @@
         <x:v/>
       </x:c>
       <x:c r="E2185" s="2" t="str">
-        <x:v>Identifies if the student has met the student growth target score</x:v>
+        <x:v>Identifies if the student growth target score is achieved.</x:v>
       </x:c>
     </x:row>
     <x:row r="2186">
@@ -39005,7 +39005,7 @@
 </x:v>
       </x:c>
       <x:c r="E2189" s="2" t="str">
-        <x:v>The target score that has been set of the group of students as it pertains to their student growth.</x:v>
+        <x:v>The target score that has been set for the group of students as it pertains to their student growth.</x:v>
       </x:c>
     </x:row>
     <x:row r="2190">
@@ -39023,7 +39023,7 @@
 </x:v>
       </x:c>
       <x:c r="E2190" s="2" t="str">
-        <x:v>The target score that has been set of the group of students as it pertains to their student growth.</x:v>
+        <x:v>The target score that has been set for the group of students as it pertains to their student growth.</x:v>
       </x:c>
     </x:row>
     <x:row r="2191">
@@ -40364,7 +40364,7 @@
 </x:v>
       </x:c>
       <x:c r="E2267" s="2" t="str">
-        <x:v>The number of student who have a disability</x:v>
+        <x:v>The number of students who have a disability.</x:v>
       </x:c>
     </x:row>
     <x:row r="2268">
@@ -44061,7 +44061,7 @@
 </x:v>
       </x:c>
       <x:c r="E2478" s="2" t="str">
-        <x:v>The percentage of student who are Title I eligible</x:v>
+        <x:v>The percentage of students who are Title I eligible.</x:v>
       </x:c>
     </x:row>
     <x:row r="2479">
@@ -44451,7 +44451,7 @@
 </x:v>
       </x:c>
       <x:c r="E2500" s="2" t="str">
-        <x:v>The percentage of student who are eligible for SchoolFoodServicesEligibility by type</x:v>
+        <x:v>The percentage of students who are eligible for SchoolFoodServicesEligibility by type.</x:v>
       </x:c>
     </x:row>
     <x:row r="2501">
@@ -46994,7 +46994,7 @@
         <x:v>EXTENSION-AggregatedNumericResponse</x:v>
       </x:c>
       <x:c r="B179" s="2" t="str">
-        <x:v>Numeric response survey data provided at the aggregate level.</x:v>
+        <x:v>The information about the numeric response for an aggregated survey.</x:v>
       </x:c>
     </x:row>
     <x:row r="180">
@@ -47098,7 +47098,7 @@
         <x:v>EXTENSION-AidTypeDescriptor</x:v>
       </x:c>
       <x:c r="B192" s="2" t="str">
-        <x:v>The classification of financial aid awarded to a person for the academic term/year.</x:v>
+        <x:v>This descriptor defines the classification of financial aid awarded to a person for the academic term/year.</x:v>
       </x:c>
     </x:row>
     <x:row r="193">
@@ -47338,7 +47338,7 @@
         <x:v>EXTENSION-BackgroundCheckTypeDescriptor</x:v>
       </x:c>
       <x:c r="B222" s="2" t="str">
-        <x:v>The type of background check (e.g., online, criminal, employment).</x:v>
+        <x:v>This descriptor defines the classification of the background check a person receives.</x:v>
       </x:c>
     </x:row>
     <x:row r="223">
@@ -47354,7 +47354,7 @@
         <x:v>EXTENSION-BoardCertification</x:v>
       </x:c>
       <x:c r="B224" s="2" t="str">
-        <x:v>Board certification information for a individual.</x:v>
+        <x:v>Board certification information for an individual.</x:v>
       </x:c>
     </x:row>
     <x:row r="225">
@@ -47362,7 +47362,7 @@
         <x:v>EXTENSION-BoardCertificationTypeDescriptor</x:v>
       </x:c>
       <x:c r="B225" s="2" t="str">
-        <x:v>The descriptor holds the  type of board certification awarded to an individual.</x:v>
+        <x:v>The descriptor holds the type of board certification awarded to an individual.</x:v>
       </x:c>
     </x:row>
     <x:row r="226">
@@ -47378,7 +47378,7 @@
         <x:v>EXTENSION-CertificationExam</x:v>
       </x:c>
       <x:c r="B227" s="2" t="str">
-        <x:v>Certification information for a individual.</x:v>
+        <x:v>Certification information for an individual.</x:v>
       </x:c>
     </x:row>
     <x:row r="228">
@@ -47386,7 +47386,7 @@
         <x:v>EXTENSION-CertificationExamTypeDescriptor</x:v>
       </x:c>
       <x:c r="B228" s="2" t="str">
-        <x:v>The descriptor holds the  type of certification exam that was taken.</x:v>
+        <x:v>The descriptor holds the type of certification exam that was taken.</x:v>
       </x:c>
     </x:row>
     <x:row r="229">
@@ -47410,7 +47410,7 @@
         <x:v>EXTENSION-CourseCourseTranscriptFacts</x:v>
       </x:c>
       <x:c r="B231" s="2" t="str">
-        <x:v>Data about the final letter grade earned of the group</x:v>
+        <x:v>Data about the final grade earned of the group.</x:v>
       </x:c>
     </x:row>
     <x:row r="232">
@@ -47594,7 +47594,7 @@
         <x:v>EXTENSION-EducationOrganizationCourseTranscriptFacts</x:v>
       </x:c>
       <x:c r="B254" s="2" t="str">
-        <x:v>Data about the final letter grade earned of the group</x:v>
+        <x:v>Data about the final grade earned of the group.</x:v>
       </x:c>
     </x:row>
     <x:row r="255">
@@ -47690,7 +47690,7 @@
         <x:v>EXTENSION-EducationOrganizationStudentFacts</x:v>
       </x:c>
       <x:c r="B266" s="2" t="str">
-        <x:v>This domain entity collects data for aggregated level students with whom the teacher candidate is associated through field work or student teaching</x:v>
+        <x:v>This domain entity collects data for aggregated level students.</x:v>
       </x:c>
     </x:row>
     <x:row r="267">
@@ -48378,7 +48378,7 @@
         <x:v>EXTENSION-SectionCourseTranscriptFacts</x:v>
       </x:c>
       <x:c r="B352" s="2" t="str">
-        <x:v>Data about the final letter grade earned of the group</x:v>
+        <x:v>Data about the final grade earned of the group.</x:v>
       </x:c>
     </x:row>
     <x:row r="353">
@@ -48402,7 +48402,7 @@
         <x:v>EXTENSION-SectionStudentAcademicRecordFacts</x:v>
       </x:c>
       <x:c r="B355" s="2" t="str">
-        <x:v>Complex type that provides data about a group of student and their academic record</x:v>
+        <x:v>Complex type that provides data about a group of students and their academic record.</x:v>
       </x:c>
     </x:row>
     <x:row r="356">
@@ -48450,7 +48450,7 @@
         <x:v>EXTENSION-SectionStudentFacts</x:v>
       </x:c>
       <x:c r="B361" s="2" t="str">
-        <x:v>This domain entity collects data for aggregated level students with whom the teacher candidate is associated through field work or student teaching</x:v>
+        <x:v>This domain entity collects data for aggregated level students.</x:v>
       </x:c>
     </x:row>
     <x:row r="362">
@@ -53698,7 +53698,7 @@
 </x:v>
       </x:c>
       <x:c r="C117" s="2" t="str">
-        <x:v>The type of background check (e.g., online, criminal, employment).</x:v>
+        <x:v>This descriptor defines the classification of the background check a person receives.</x:v>
       </x:c>
     </x:row>
     <x:row r="118">
@@ -53711,7 +53711,7 @@
 Art/Early and Middle Childhood
 Career and Technical Education/Early Adolescence through Young Adulthood
 English as a New Language/Early Adolescence through Young Adulthood
-English as  New Language/Early and Middle Childhood
+English as a New Language/Early and Middle Childhood
 English Language Arts/Adolescence and Young Adulthood
 English Language Arts/Early Adolescence
 Exceptional Needs Specialist/Early Childhood through Young Adulthood
@@ -53738,7 +53738,7 @@
 </x:v>
       </x:c>
       <x:c r="C118" s="2" t="str">
-        <x:v>Map for the board certiciation board types.</x:v>
+        <x:v>Map for the board certification board types.</x:v>
       </x:c>
     </x:row>
     <x:row r="119">
@@ -53792,7 +53792,7 @@
 </x:v>
       </x:c>
       <x:c r="C122" s="2" t="str">
-        <x:v>Indicates that a person passed, failed, or did not take an English Language assessment (e.g., TOEFFL).</x:v>
+        <x:v>The rating the individual received on the English Language assessment.</x:v>
       </x:c>
     </x:row>
     <x:row r="123">

</xml_diff>

<commit_message>
Updates to more clearly delineate TPDP Extensions to TNTP
</commit_message>
<xml_diff>
--- a/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
+++ b/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
@@ -2723,7 +2723,7 @@
 </x:v>
       </x:c>
       <x:c r="E146" s="2" t="str">
-        <x:v>(TPDP Extension) Salary information collected at the aggregate level.</x:v>
+        <x:v>Salary information collected at the aggregate level.</x:v>
       </x:c>
     </x:row>
     <x:row r="147">
@@ -3202,7 +3202,7 @@
 </x:v>
       </x:c>
       <x:c r="E172" s="2" t="str">
-        <x:v>(TPDP Extension) This entity represents the financial aid a person is awarded.</x:v>
+        <x:v>This entity represents the financial aid a person is awarded.</x:v>
       </x:c>
     </x:row>
     <x:row r="173">
@@ -6267,7 +6267,7 @@
 </x:v>
       </x:c>
       <x:c r="E342" s="2" t="str">
-        <x:v>(TPDP Extension) The average number of years that all staff have been employed in the current district of employment.</x:v>
+        <x:v>The average number of years that all staff have been employed in the current district of employment.</x:v>
       </x:c>
     </x:row>
     <x:row r="343">
@@ -10558,7 +10558,7 @@
 </x:v>
       </x:c>
       <x:c r="E585" s="2" t="str">
-        <x:v>(TPDP Extension) The course associated with the survey.</x:v>
+        <x:v>The course associated with the survey.</x:v>
       </x:c>
     </x:row>
     <x:row r="586">
@@ -11250,7 +11250,7 @@
 </x:v>
       </x:c>
       <x:c r="E624" s="2" t="str">
-        <x:v>(TPDP Extension) The legal document or authorization giving authorization to perform teaching assignment services.</x:v>
+        <x:v>The legal document or authorization giving authorization to perform teaching assignment services.</x:v>
       </x:c>
     </x:row>
     <x:row r="625">
@@ -12760,7 +12760,7 @@
 </x:v>
       </x:c>
       <x:c r="E708" s="2" t="str">
-        <x:v>(TPDP Extension) The disability condition(s) that best describes an individual's impairment.</x:v>
+        <x:v>The disability condition(s) that best describes an individual's impairment.</x:v>
       </x:c>
     </x:row>
     <x:row r="709">
@@ -12779,7 +12779,7 @@
 </x:v>
       </x:c>
       <x:c r="E709" s="2" t="str">
-        <x:v>(TPDP Extension) The disability condition(s) that best describes an individual's impairment.</x:v>
+        <x:v>The disability condition(s) that best describes an individual's impairment.</x:v>
       </x:c>
     </x:row>
     <x:row r="710">
@@ -15097,7 +15097,7 @@
 </x:v>
       </x:c>
       <x:c r="E841" s="2" t="str">
-        <x:v>(TPDP Change) The Education Organization(s) associated with the survey.</x:v>
+        <x:v>The Education Organization(s) associated with the survey.</x:v>
       </x:c>
     </x:row>
     <x:row r="842">
@@ -17672,7 +17672,7 @@
 </x:v>
       </x:c>
       <x:c r="E986" s="2" t="str">
-        <x:v>(TPDP Extension) The location of the event.</x:v>
+        <x:v>The location of the event.</x:v>
       </x:c>
     </x:row>
     <x:row r="987">
@@ -19315,7 +19315,7 @@
 </x:v>
       </x:c>
       <x:c r="E1081" s="2" t="str">
-        <x:v>(TPDP Extension) Indicates that a person has or has not completed a fingerprint.</x:v>
+        <x:v>Indicates that a person has or has not completed a fingerprint.</x:v>
       </x:c>
     </x:row>
     <x:row r="1082">
@@ -19524,7 +19524,7 @@
 </x:v>
       </x:c>
       <x:c r="E1093" s="2" t="str">
-        <x:v>(TPDP Extension) The gender with which a person associates.</x:v>
+        <x:v>The gender with which a person associates.</x:v>
       </x:c>
     </x:row>
     <x:row r="1094">
@@ -19542,7 +19542,7 @@
 </x:v>
       </x:c>
       <x:c r="E1094" s="2" t="str">
-        <x:v>(TPDP Extension) The gender with which a person associates.</x:v>
+        <x:v>The gender with which a person associates.</x:v>
       </x:c>
     </x:row>
     <x:row r="1095">
@@ -21085,7 +21085,7 @@
 </x:v>
       </x:c>
       <x:c r="E1181" s="2" t="str">
-        <x:v>(TPDP Extension) The percent of staff hired for the education organization.</x:v>
+        <x:v>The percent of staff hired for the education organization.</x:v>
       </x:c>
     </x:row>
     <x:row r="1182">
@@ -24830,7 +24830,7 @@
 </x:v>
       </x:c>
       <x:c r="E1390" s="2" t="str">
-        <x:v>(TPDP Extension) Information about the matrix element in the survey</x:v>
+        <x:v>Information about the matrix element in the survey</x:v>
       </x:c>
     </x:row>
     <x:row r="1391">
@@ -29744,7 +29744,7 @@
 </x:v>
       </x:c>
       <x:c r="E1664" s="2" t="str">
-        <x:v>(TPDP Extension) The program associated with the survey.</x:v>
+        <x:v>The program associated with the survey.</x:v>
       </x:c>
     </x:row>
     <x:row r="1665">
@@ -30147,7 +30147,7 @@
 </x:v>
       </x:c>
       <x:c r="E1687" s="2" t="str">
-        <x:v>(TPDP Extension) The qualifications of a prospective mentor teacher.</x:v>
+        <x:v>The qualifications of a prospective mentor teacher.</x:v>
       </x:c>
     </x:row>
     <x:row r="1688">
@@ -30182,7 +30182,7 @@
         <x:v/>
       </x:c>
       <x:c r="E1689" s="2" t="str">
-        <x:v>(TPDP Extension) The reference to the prospect.</x:v>
+        <x:v>The reference to the prospect.</x:v>
       </x:c>
     </x:row>
     <x:row r="1690">
@@ -31888,7 +31888,7 @@
 </x:v>
       </x:c>
       <x:c r="E1783" s="2" t="str">
-        <x:v>(TPDP Extension) The percent of staff retained for the education organization.</x:v>
+        <x:v>The percent of staff retained for the education organization.</x:v>
       </x:c>
     </x:row>
     <x:row r="1784">
@@ -31928,7 +31928,7 @@
 </x:v>
       </x:c>
       <x:c r="E1785" s="2" t="str">
-        <x:v>(TPDP Extension) The percent of staff retired for the education organization.</x:v>
+        <x:v>The percent of staff retired for the education organization.</x:v>
       </x:c>
     </x:row>
     <x:row r="1786">
@@ -34209,7 +34209,7 @@
 </x:v>
       </x:c>
       <x:c r="E1916" s="2" t="str">
-        <x:v>(TPDP Extension) A meaningful score or statistical expression of the performance of an individual. The results can be expressed as a number, percentile, range, level, etc.</x:v>
+        <x:v>A meaningful score or statistical expression of the performance of an individual. The results can be expressed as a number, percentile, range, level, etc.</x:v>
       </x:c>
     </x:row>
     <x:row r="1917">
@@ -34512,7 +34512,7 @@
 </x:v>
       </x:c>
       <x:c r="E1933" s="2" t="str">
-        <x:v>(TPDP Extension) The section associated with the survey.</x:v>
+        <x:v>The section associated with the survey.</x:v>
       </x:c>
     </x:row>
     <x:row r="1934">
@@ -44161,7 +44161,7 @@
 </x:v>
       </x:c>
       <x:c r="E2482" s="2" t="str">
-        <x:v>(TPDP Extension) This entity represents actual and projected vacancies for the education organization.</x:v>
+        <x:v>This entity represents actual and projected vacancies for the education organization.</x:v>
       </x:c>
     </x:row>
     <x:row r="2483">

</xml_diff>

<commit_message>
Lengths from older buggy notations changed
</commit_message>
<xml_diff>
--- a/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
+++ b/MetaEdOutput/DataDictionary/Public-Ed-Fi-XML-Data-Dictionary.xlsx
@@ -53370,8 +53370,7 @@
         <x:v>EXTENSION-LevelTitle</x:v>
       </x:c>
       <x:c r="B134" s="2" t="str">
-        <x:v>minLength: 2
-maxLength: 15
+        <x:v>maxLength: 60
 </x:v>
       </x:c>
       <x:c r="C134" s="2" t="str">
@@ -53693,8 +53692,7 @@
         <x:v>EXTENSION-RubricTitle</x:v>
       </x:c>
       <x:c r="B157" s="2" t="str">
-        <x:v>minLength: 2
-maxLength: 15
+        <x:v>maxLength: 60
 </x:v>
       </x:c>
       <x:c r="C157" s="2" t="str">

</xml_diff>